<commit_message>
perform payment via entering the account number
</commit_message>
<xml_diff>
--- a/new_payment.xlsx
+++ b/new_payment.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">Emetteur</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">Compte Emetteur</t>
   </si>
   <si>
     <t xml:space="preserve">Bénéficiaire</t>
@@ -40,10 +40,10 @@
     <t xml:space="preserve">Date désirée</t>
   </si>
   <si>
-    <t xml:space="preserve">NjczODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NjczODA</t>
+    <t xml:space="preserve">BE39914001921319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR1130002005440000007765L61</t>
   </si>
   <si>
     <t xml:space="preserve">jjj</t>
@@ -52,16 +52,19 @@
     <t xml:space="preserve">opoo</t>
   </si>
   <si>
+    <t xml:space="preserve">BE17914001921521</t>
+  </si>
+  <si>
     <t xml:space="preserve">ha</t>
   </si>
   <si>
     <t xml:space="preserve">euh</t>
   </si>
   <si>
-    <t xml:space="preserve">FXBBBEBBXXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BKTWTWTP223</t>
+    <t xml:space="preserve">BE12914005042392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS35155000000000563774</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -158,10 +161,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,26 +194,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1015560</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>393120</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
-    </xdr:to>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -312,116 +307,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="223" zoomScaleNormal="223" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.74"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+    <row r="1" s="4" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>45705</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>223007103689</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>45706</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>45705</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>45706</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -430,9 +397,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
qui paie les  frais de tranfert
</commit_message>
<xml_diff>
--- a/new_payment.xlsx
+++ b/new_payment.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Compte Emetteur</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">Expéditeur</t>
   </si>
   <si>
     <t xml:space="preserve">Bénéficiaire</t>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Montant</t>
   </si>
   <si>
-    <t xml:space="preserve">Libélé</t>
+    <t xml:space="preserve">Libellé</t>
   </si>
   <si>
     <t xml:space="preserve">Commentaire</t>
@@ -40,31 +40,40 @@
     <t xml:space="preserve">Date désirée</t>
   </si>
   <si>
+    <t xml:space="preserve">Détails des frais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urgence</t>
+  </si>
+  <si>
     <t xml:space="preserve">BE39914001921319</t>
   </si>
   <si>
     <t xml:space="preserve">FR1130002005440000007765L61</t>
   </si>
   <si>
-    <t xml:space="preserve">jjj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opoo</t>
+    <t xml:space="preserve">there is the tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this the comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">our</t>
   </si>
   <si>
     <t xml:space="preserve">BE17914001921521</t>
   </si>
   <si>
-    <t xml:space="preserve">ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">euh</t>
+    <t xml:space="preserve">RS35160005010008573607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ben</t>
   </si>
   <si>
     <t xml:space="preserve">BE12914005042392</t>
   </si>
   <si>
-    <t xml:space="preserve">RS35155000000000563774</t>
+    <t xml:space="preserve">09cf660e9747a34</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,24 +109,34 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEDCE6"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800080"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -126,6 +144,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -152,40 +191,72 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -198,6 +269,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDEDCE6"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -312,88 +443,104 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="223" zoomScaleNormal="223" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="9" style="5" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="9" customFormat="true" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="12" t="n">
         <v>14</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>45705</v>
+      <c r="D2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>45708</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="12" t="n">
+        <v>24</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="n">
-        <v>223007103689</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>45706</v>
+      <c r="F3" s="3" t="n">
+        <v>45709</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="A4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="16" t="n">
         <v>21</v>
       </c>
     </row>

</xml_diff>